<commit_message>
updates and DO work
</commit_message>
<xml_diff>
--- a/N_uptake_NEON/data/NEON_no3sensor_locations.xlsx
+++ b/N_uptake_NEON/data/NEON_no3sensor_locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torrensc/Documents/R_working/Modelscape/space-time-rivers/N_uptake_NEON/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB636723-8506-D542-9D71-026E9A2DB3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DD1E52-7C68-D54B-8EBE-86CB365E2F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="960" windowWidth="19380" windowHeight="14380" firstSheet="1" activeTab="1" xr2:uid="{A66FB1EE-F6D3-844E-A266-EAF15830FFBA}"/>
+    <workbookView xWindow="4480" yWindow="680" windowWidth="19380" windowHeight="14380" firstSheet="1" activeTab="1" xr2:uid="{A66FB1EE-F6D3-844E-A266-EAF15830FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="NEON_no3sensor_locations" sheetId="1" r:id="rId1"/>
@@ -3577,22 +3577,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91305569-FDC5-9540-B8A6-370A2C965CC6}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="34" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="35.33203125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="9" max="13" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" hidden="1" customWidth="1"/>
-    <col min="15" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="17" max="22" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
+    <col min="15" max="23" width="10.83203125" customWidth="1"/>
     <col min="24" max="24" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
clean up proj files; remove poorly modeled days; rerun all models
clean up proj files; remove poorly modeled days; rerun all models
</commit_message>
<xml_diff>
--- a/N_uptake_NEON/data/NEON_no3sensor_locations.xlsx
+++ b/N_uptake_NEON/data/NEON_no3sensor_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torrensc/Documents/R_working/Modelscape/space-time-rivers/N_uptake_NEON/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DD1E52-7C68-D54B-8EBE-86CB365E2F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E16D9E2-EE3B-3443-9A0C-EE809FBC5409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="680" windowWidth="19380" windowHeight="14380" firstSheet="1" activeTab="1" xr2:uid="{A66FB1EE-F6D3-844E-A266-EAF15830FFBA}"/>
+    <workbookView xWindow="4480" yWindow="760" windowWidth="19380" windowHeight="14380" firstSheet="1" activeTab="1" xr2:uid="{A66FB1EE-F6D3-844E-A266-EAF15830FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="NEON_no3sensor_locations" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="244">
   <si>
     <t>siteID</t>
   </si>
@@ -757,6 +757,15 @@
   </si>
   <si>
     <t>K (d^-1)</t>
+  </si>
+  <si>
+    <t>Lat_locationReferenceLatitude</t>
+  </si>
+  <si>
+    <t>Long_locationReferenceLongitude</t>
+  </si>
+  <si>
+    <t>Elev_locationReferenceElevation</t>
   </si>
 </sst>
 </file>
@@ -3577,8 +3586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91305569-FDC5-9540-B8A6-370A2C965CC6}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="B5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3626,13 +3635,13 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>241</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>242</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>243</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -4021,7 +4030,9 @@
       <c r="AG5" s="8"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="B6" s="8" t="s">
         <v>193</v>
       </c>
@@ -4168,6 +4179,9 @@
       <c r="AG7" s="9"/>
     </row>
     <row r="8" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>182</v>
+      </c>
       <c r="B8" s="8" t="s">
         <v>76</v>
       </c>

</xml_diff>